<commit_message>
Criação da classe de identificação de tipos
</commit_message>
<xml_diff>
--- a/df_teste.xlsx
+++ b/df_teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biral\Documents\Identificador Aumotatico Colunas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2C163F-A75D-4C88-8C05-9D17E398165A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55010300-6E5A-404E-AF04-63F716ECEFD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F098D2FD-3C99-4202-8313-A67173136B14}"/>
   </bookViews>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">_xlfn.CONCAT(TRUNC(100*RAND(),0),"9",TRUNC(100000000*RAND(),0))</f>
-        <v>82930632571</v>
+        <v>8916052855</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -3240,7 +3240,7 @@
       </c>
       <c r="C3">
         <f ca="1">TRUNC(100000000*RAND(),0)</f>
-        <v>8619429</v>
+        <v>92989001</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>